<commit_message>
Report: normalised results plot.
</commit_message>
<xml_diff>
--- a/report/plots/Excel/graphs.xlsx
+++ b/report/plots/Excel/graphs.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\Uni\Dropbox\COMP4620\Assignments\prac\aixi\report\plots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Uni\Dropbox\COMP4620\Assignments\prac\aixi\report\plots\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="kpok" sheetId="1" r:id="rId1"/>
     <sheet name="pacman" sheetId="2" r:id="rId2"/>
     <sheet name="rps" sheetId="3" r:id="rId3"/>
     <sheet name="tiger" sheetId="4" r:id="rId4"/>
+    <sheet name="Comparison" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Cycles</t>
   </si>
@@ -39,6 +40,27 @@
   </si>
   <si>
     <t>Optimal</t>
+  </si>
+  <si>
+    <t>kpok</t>
+  </si>
+  <si>
+    <t>pacman</t>
+  </si>
+  <si>
+    <t>rps</t>
+  </si>
+  <si>
+    <t>tiger</t>
+  </si>
+  <si>
+    <t>Opt</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>optimal</t>
   </si>
 </sst>
 </file>
@@ -130,7 +152,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -334,11 +355,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="467123152"/>
-        <c:axId val="467110640"/>
+        <c:axId val="127207488"/>
+        <c:axId val="127210208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="467123152"/>
+        <c:axId val="127207488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -367,7 +388,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -423,7 +443,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467110640"/>
+        <c:crossAx val="127210208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -431,7 +451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="467110640"/>
+        <c:axId val="127210208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -460,7 +480,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -515,7 +534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467123152"/>
+        <c:crossAx val="127207488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -531,7 +550,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -631,7 +649,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -879,11 +896,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="467111184"/>
-        <c:axId val="467121520"/>
+        <c:axId val="127204768"/>
+        <c:axId val="127212384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="467111184"/>
+        <c:axId val="127204768"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -915,7 +932,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -971,12 +987,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467121520"/>
+        <c:crossAx val="127212384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="467121520"/>
+        <c:axId val="127212384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1005,7 +1021,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1060,7 +1075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467111184"/>
+        <c:crossAx val="127204768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1076,7 +1091,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1176,7 +1190,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1323,11 +1336,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="467112816"/>
-        <c:axId val="467122064"/>
+        <c:axId val="127208576"/>
+        <c:axId val="127215104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="467112816"/>
+        <c:axId val="127208576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1356,7 +1369,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1412,7 +1424,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467122064"/>
+        <c:crossAx val="127215104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1420,7 +1432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="467122064"/>
+        <c:axId val="127215104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-1"/>
@@ -1450,7 +1462,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1505,7 +1516,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467112816"/>
+        <c:crossAx val="127208576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1592,7 +1603,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1796,11 +1806,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="467118256"/>
-        <c:axId val="467112272"/>
+        <c:axId val="127212928"/>
+        <c:axId val="127213472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="467118256"/>
+        <c:axId val="127212928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1829,7 +1839,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1885,7 +1894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467112272"/>
+        <c:crossAx val="127213472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1893,7 +1902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="467112272"/>
+        <c:axId val="127213472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.30000000000000004"/>
@@ -1924,7 +1933,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1979,7 +1987,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467118256"/>
+        <c:crossAx val="127212928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1995,7 +2003,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2095,7 +2102,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2299,11 +2305,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="467113904"/>
-        <c:axId val="467114448"/>
+        <c:axId val="127203136"/>
+        <c:axId val="127203680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="467113904"/>
+        <c:axId val="127203136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2332,7 +2338,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2388,7 +2393,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467114448"/>
+        <c:crossAx val="127203680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2396,7 +2401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="467114448"/>
+        <c:axId val="127203680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2425,7 +2430,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2480,7 +2484,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467113904"/>
+        <c:crossAx val="127203136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2490,6 +2494,877 @@
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Normalised  Reward</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>kpok</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Comparison!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Comparison!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.96363243243243246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9646054054054054</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95166972972972985</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95283729729729738</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96421621621621634</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97394594594594597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98143783783783789</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9812432432432433</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99719513513513514</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>pacman</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Comparison!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Comparison!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.88871875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88981250000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89387499999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88325468750000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90284374999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90721093750000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92184374999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.91828125000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>rps</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Comparison!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Comparison!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.97724800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95788799999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97052800000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96300799999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96716800000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98843999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97932799999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98108000000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97548800000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>tiger</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Comparison!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Comparison!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.97675201155966385</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98071080056610682</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99164695519640544</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9929038707059511</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99580368365317062</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99190427648182422</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99162716125137318</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9927554161182095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99302263437614435</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Optimal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Comparison!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Comparison!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="90828528"/>
+        <c:axId val="2103723072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="90828528"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:min val="512"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Experience</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2103723072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2103723072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.02"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Average Reward per Cycle</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="90828528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -2759,6 +3634,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -5320,6 +6235,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -5517,6 +6948,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>364192</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>287992</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>173691</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5783,7 +7249,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5960,7 +7426,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6265,8 +7731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6427,4 +7893,291 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>512</v>
+      </c>
+      <c r="B2">
+        <f>kpok!B2/($B$12+$B$13)</f>
+        <v>0.96363243243243246</v>
+      </c>
+      <c r="C2">
+        <f>pacman!B2/($C$12+$C$13)</f>
+        <v>0.88871875</v>
+      </c>
+      <c r="D2">
+        <f>rps!B2/($D$12+$D$13)</f>
+        <v>0.97724800000000001</v>
+      </c>
+      <c r="E2">
+        <f>tiger!B2/($E$12+$E$13)</f>
+        <v>0.97675201155966385</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1024</v>
+      </c>
+      <c r="B3">
+        <f>kpok!B3/($B$12+$B$13)</f>
+        <v>0.9646054054054054</v>
+      </c>
+      <c r="C3">
+        <f>pacman!B3/($C$12+$C$13)</f>
+        <v>0.88981250000000001</v>
+      </c>
+      <c r="D3">
+        <f>rps!B3/($D$12+$D$13)</f>
+        <v>0.95788799999999996</v>
+      </c>
+      <c r="E3">
+        <f>tiger!B3/($E$12+$E$13)</f>
+        <v>0.98071080056610682</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2048</v>
+      </c>
+      <c r="B4">
+        <f>kpok!B4/($B$12+$B$13)</f>
+        <v>0.95166972972972985</v>
+      </c>
+      <c r="C4">
+        <f>pacman!B4/($C$12+$C$13)</f>
+        <v>0.89387499999999998</v>
+      </c>
+      <c r="D4">
+        <f>rps!B4/($D$12+$D$13)</f>
+        <v>0.97052800000000006</v>
+      </c>
+      <c r="E4">
+        <f>tiger!B4/($E$12+$E$13)</f>
+        <v>0.99164695519640544</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4096</v>
+      </c>
+      <c r="B5">
+        <f>kpok!B5/($B$12+$B$13)</f>
+        <v>0.95283729729729738</v>
+      </c>
+      <c r="C5">
+        <f>pacman!B5/($C$12+$C$13)</f>
+        <v>0.88325468750000002</v>
+      </c>
+      <c r="D5">
+        <f>rps!B5/($D$12+$D$13)</f>
+        <v>0.96300799999999998</v>
+      </c>
+      <c r="E5">
+        <f>tiger!B5/($E$12+$E$13)</f>
+        <v>0.9929038707059511</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8192</v>
+      </c>
+      <c r="B6">
+        <f>kpok!B6/($B$12+$B$13)</f>
+        <v>0.96421621621621634</v>
+      </c>
+      <c r="C6">
+        <f>pacman!B6/($C$12+$C$13)</f>
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="D6">
+        <f>rps!B6/($D$12+$D$13)</f>
+        <v>0.96716800000000003</v>
+      </c>
+      <c r="E6">
+        <f>tiger!B6/($E$12+$E$13)</f>
+        <v>0.99580368365317062</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>16384</v>
+      </c>
+      <c r="B7">
+        <f>kpok!B7/($B$12+$B$13)</f>
+        <v>0.97394594594594597</v>
+      </c>
+      <c r="C7">
+        <f>pacman!B7/($C$12+$C$13)</f>
+        <v>0.90284374999999994</v>
+      </c>
+      <c r="D7">
+        <f>rps!B7/($D$12+$D$13)</f>
+        <v>0.98843999999999999</v>
+      </c>
+      <c r="E7">
+        <f>tiger!B7/($E$12+$E$13)</f>
+        <v>0.99190427648182422</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>32768</v>
+      </c>
+      <c r="B8">
+        <f>kpok!B8/($B$12+$B$13)</f>
+        <v>0.98143783783783789</v>
+      </c>
+      <c r="C8">
+        <f>pacman!B8/($C$12+$C$13)</f>
+        <v>0.90721093750000004</v>
+      </c>
+      <c r="D8">
+        <f>rps!B8/($D$12+$D$13)</f>
+        <v>0.97932799999999998</v>
+      </c>
+      <c r="E8">
+        <f>tiger!B8/($E$12+$E$13)</f>
+        <v>0.99162716125137318</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>65536</v>
+      </c>
+      <c r="B9">
+        <f>kpok!B9/($B$12+$B$13)</f>
+        <v>0.9812432432432433</v>
+      </c>
+      <c r="C9">
+        <f>pacman!B9/($C$12+$C$13)</f>
+        <v>0.92184374999999996</v>
+      </c>
+      <c r="D9">
+        <f>rps!B9/($D$12+$D$13)</f>
+        <v>0.98108000000000006</v>
+      </c>
+      <c r="E9">
+        <f>tiger!B9/($E$12+$E$13)</f>
+        <v>0.9927554161182095</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100000</v>
+      </c>
+      <c r="B10">
+        <f>kpok!B10/($B$12+$B$13)</f>
+        <v>0.99719513513513514</v>
+      </c>
+      <c r="C10">
+        <f>pacman!B10/($C$12+$C$13)</f>
+        <v>0.91828125000000005</v>
+      </c>
+      <c r="D10">
+        <f>rps!B10/($D$12+$D$13)</f>
+        <v>0.97548800000000002</v>
+      </c>
+      <c r="E10">
+        <f>tiger!B10/($E$12+$E$13)</f>
+        <v>0.99302263437614435</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <f>1/18</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0.25</v>
+      </c>
+      <c r="E12">
+        <v>1.0409999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>61</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>